<commit_message>
update the sample size table after the sample filtration in ffa26d795c475408e3d0e78f2a81dcdb740875ca
</commit_message>
<xml_diff>
--- a/data/processed/tbl-sample-sizes.xlsx
+++ b/data/processed/tbl-sample-sizes.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Dessert</t>
   </si>
@@ -23,34 +23,37 @@
     <t>French</t>
   </si>
   <si>
-    <t>Acidity</t>
-  </si>
-  <si>
-    <t>DeltaAcidity</t>
-  </si>
-  <si>
-    <t>SSC</t>
-  </si>
-  <si>
-    <t>Firmness</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Juiciness</t>
-  </si>
-  <si>
-    <t>PhenolicContent</t>
-  </si>
-  <si>
-    <t>HarvestDate</t>
-  </si>
-  <si>
-    <t>FloweringDate</t>
-  </si>
-  <si>
-    <t>Softening</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
         <v>11.0</v>
       </c>
       <c r="D2" t="n">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="3">
@@ -135,10 +138,10 @@
         <v>14.0</v>
       </c>
       <c r="C3" t="n">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="D3" t="n">
-        <v>20.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="4">
@@ -146,13 +149,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C4" t="n">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="D4" t="n">
-        <v>29.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="5">
@@ -160,7 +163,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C5" t="n">
         <v>11.0</v>
@@ -174,7 +177,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C6" t="n">
         <v>11.0</v>
@@ -188,13 +191,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="C7" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D7" t="n">
-        <v>17.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="8">
@@ -202,13 +205,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D8" t="n">
         <v>13.0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>17.0</v>
       </c>
     </row>
     <row r="9">
@@ -216,13 +219,13 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="C9" t="n">
-        <v>12.0</v>
+        <v>3.0</v>
       </c>
       <c r="D9" t="n">
-        <v>18.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="10">
@@ -230,13 +233,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="C10" t="n">
-        <v>26.0</v>
+        <v>11.0</v>
       </c>
       <c r="D10" t="n">
-        <v>42.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="11">
@@ -244,12 +247,26 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>12.0</v>
+        <v>14.0</v>
       </c>
       <c r="C11" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C12" t="n">
         <v>7.0</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D12" t="n">
         <v>23.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finalize the data curation
</commit_message>
<xml_diff>
--- a/data/processed/tbl-sample-sizes.xlsx
+++ b/data/processed/tbl-sample-sizes.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Dessert</t>
   </si>
@@ -23,37 +23,34 @@
     <t>French</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
+    <t>Acidity</t>
+  </si>
+  <si>
+    <t>DeltaAcidity</t>
+  </si>
+  <si>
+    <t>SSC</t>
+  </si>
+  <si>
+    <t>Firmness</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Juiciness</t>
+  </si>
+  <si>
+    <t>PhenolicContent</t>
+  </si>
+  <si>
+    <t>HarvestDate</t>
+  </si>
+  <si>
+    <t>FloweringDate</t>
+  </si>
+  <si>
+    <t>Softening</t>
   </si>
 </sst>
 </file>
@@ -124,10 +121,10 @@
         <v>14.0</v>
       </c>
       <c r="C2" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D2" t="n">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="3">
@@ -138,10 +135,10 @@
         <v>14.0</v>
       </c>
       <c r="C3" t="n">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="D3" t="n">
-        <v>28.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="4">
@@ -149,13 +146,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="C4" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="D4" t="n">
-        <v>20.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="5">
@@ -163,10 +160,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="C5" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D5" t="n">
         <v>29.0</v>
@@ -177,10 +174,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="C6" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D6" t="n">
         <v>29.0</v>
@@ -191,13 +188,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
       <c r="C7" t="n">
-        <v>11.0</v>
+        <v>5.0</v>
       </c>
       <c r="D7" t="n">
-        <v>29.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="8">
@@ -208,10 +205,10 @@
         <v>12.0</v>
       </c>
       <c r="C8" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="D8" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="9">
@@ -219,13 +216,13 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
       <c r="C9" t="n">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
       <c r="D9" t="n">
-        <v>12.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="10">
@@ -233,10 +230,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
       <c r="C10" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D10" t="n">
         <v>29.0</v>
@@ -247,26 +244,12 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
       <c r="C11" t="n">
-        <v>11.0</v>
+        <v>6.0</v>
       </c>
       <c r="D11" t="n">
-        <v>29.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="D12" t="n">
         <v>23.0</v>
       </c>
     </row>

</xml_diff>